<commit_message>
Update requirements stack Final Sprint
</commit_message>
<xml_diff>
--- a/documentation/User_Stories_and_Requirements_Stack.xlsx
+++ b/documentation/User_Stories_and_Requirements_Stack.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Reference Story No.</t>
   </si>
@@ -257,7 +257,7 @@
     <t>Let admin delete items</t>
   </si>
   <si>
-    <t>Add privacy policy and terms</t>
+    <t>Fix server console warnings</t>
   </si>
   <si>
     <t>Test login and progress features</t>
@@ -275,10 +275,10 @@
     <t>Final general UI testing</t>
   </si>
   <si>
+    <t>Write final presentation document</t>
+  </si>
+  <si>
     <t>Prepare demo and presentation</t>
-  </si>
-  <si>
-    <t>Write final report and notes</t>
   </si>
 </sst>
 </file>
@@ -521,6 +521,12 @@
         <bottom style="thin">
           <color rgb="FF356854"/>
         </bottom>
+        <vertical style="thin">
+          <color rgb="FFD4D4D4"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FFD4D4D4"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -1903,6 +1909,9 @@
       <c r="E38" s="23">
         <v>4.0</v>
       </c>
+      <c r="G38" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="21">
@@ -1920,6 +1929,9 @@
       <c r="E39" s="23">
         <v>4.0</v>
       </c>
+      <c r="G39" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="23">
@@ -1937,6 +1949,9 @@
       <c r="E40" s="23">
         <v>4.0</v>
       </c>
+      <c r="G40" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="21">
@@ -1954,6 +1969,9 @@
       <c r="E41" s="23">
         <v>4.0</v>
       </c>
+      <c r="G41" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="23">
@@ -1971,6 +1989,9 @@
       <c r="E42" s="23">
         <v>4.0</v>
       </c>
+      <c r="G42" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="21">
@@ -1988,12 +2009,15 @@
       <c r="E43" s="23">
         <v>4.0</v>
       </c>
+      <c r="G43" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="23">
         <v>43.0</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="10" t="s">
         <v>87</v>
       </c>
       <c r="C44" s="23">
@@ -2004,6 +2028,9 @@
       </c>
       <c r="E44" s="23">
         <v>4.0</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="45">
@@ -2021,6 +2048,9 @@
       </c>
       <c r="E45" s="23">
         <v>4.0</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>